<commit_message>
More parts of Scenario tag loaded, update readme with 2019-12 progress
</commit_message>
<xml_diff>
--- a/doc/Research/ScenarioResearch.xlsx
+++ b/doc/Research/ScenarioResearch.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronal\source\openh2\doc\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A8830-4E30-4EF1-B37F-EEFCAE68A064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F124A0C7-275F-43DA-814C-EE35F9617AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2 (2)" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Scripting" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="MixedRefs">Sheet1!$B$2:$F$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
   <si>
     <t>Cao Location</t>
   </si>
@@ -165,9 +165,6 @@
     <t>player spawn, xyz with rotation - almost certainly</t>
   </si>
   <si>
-    <t>definitely sword placement on zanzibar - but not on lockout, no shotgun on lockout either</t>
-  </si>
-  <si>
     <t>Crates and stuff</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>ammo pickups</t>
   </si>
   <si>
-    <t>machine placement</t>
-  </si>
-  <si>
     <t>Vehi references</t>
   </si>
   <si>
@@ -271,6 +265,108 @@
   </si>
   <si>
     <t>Some shorts</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>equipment refs</t>
+  </si>
+  <si>
+    <t>mach placement</t>
+  </si>
+  <si>
+    <t>vehicle refs</t>
+  </si>
+  <si>
+    <t>Obj440s seem like entry points</t>
+  </si>
+  <si>
+    <t>Obj568 seem like script nodes</t>
+  </si>
+  <si>
+    <t>Obj568's ValueE might be "next node"</t>
+  </si>
+  <si>
+    <t>ValueA</t>
+  </si>
+  <si>
+    <t>ValueB</t>
+  </si>
+  <si>
+    <t>ValueC</t>
+  </si>
+  <si>
+    <t>ValueD</t>
+  </si>
+  <si>
+    <t>ValueE</t>
+  </si>
+  <si>
+    <t>ValueF</t>
+  </si>
+  <si>
+    <t>ValueG</t>
+  </si>
+  <si>
+    <t>ValueH</t>
+  </si>
+  <si>
+    <t>ValueI</t>
+  </si>
+  <si>
+    <t>ValueJ</t>
+  </si>
+  <si>
+    <t>next node</t>
+  </si>
+  <si>
+    <t>Obj440</t>
+  </si>
+  <si>
+    <t>an index into Obj568</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> large, always matches with Obj568 ValueA, sometimes ValueG</t>
+  </si>
+  <si>
+    <t>Index1</t>
+  </si>
+  <si>
+    <t>always (0,1,3,5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index2 </t>
+  </si>
+  <si>
+    <t>(4,5,7,51)</t>
+  </si>
+  <si>
+    <t>large, matches ValueB from Obj440</t>
+  </si>
+  <si>
+    <t>Values between 0-897</t>
+  </si>
+  <si>
+    <t>values between 0-56</t>
+  </si>
+  <si>
+    <t>(0,1,8,9,10,13) flags?</t>
+  </si>
+  <si>
+    <t>Only short.MaxValue -&gt; ushort.MaxValue, maybe actually two separate byte values?</t>
+  </si>
+  <si>
+    <t>0 -&gt; ushort.MaxValue</t>
+  </si>
+  <si>
+    <t>(0,1,2,3,4)</t>
+  </si>
+  <si>
+    <t>Mostly 0-20900ish, last hundred or so go up to around ushort.MaxValue</t>
+  </si>
+  <si>
+    <t>Some lower values, but mostly 32k and up, maybe separate byte vals</t>
   </si>
 </sst>
 </file>
@@ -388,8 +484,56 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7979"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -700,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1D70A5-77EB-4101-A684-C29A663B6757}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +951,7 @@
         <v>92</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="1"/>
@@ -852,7 +996,7 @@
         <v>120</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="2"/>
@@ -864,7 +1008,7 @@
         <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
@@ -914,8 +1058,8 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>42</v>
+      <c r="F9" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
@@ -1070,7 +1214,7 @@
         <v>248</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
@@ -1250,7 +1394,7 @@
         <v>336</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="2"/>
@@ -1262,7 +1406,7 @@
         <v>344</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
@@ -1274,7 +1418,7 @@
         <v>352</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
@@ -1286,7 +1430,7 @@
         <v>360</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
@@ -1298,7 +1442,7 @@
         <v>368</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
@@ -1310,7 +1454,7 @@
         <v>376</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
@@ -1335,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
@@ -1354,7 +1498,7 @@
         <v>456</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
@@ -1376,7 +1520,7 @@
         <v>128</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="1"/>
@@ -1499,7 +1643,7 @@
         <v>576</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="2"/>
@@ -1540,7 +1684,7 @@
         <v>584</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
@@ -1646,7 +1790,7 @@
         <v>76</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -1691,7 +1835,7 @@
         <v>832</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="2"/>
@@ -1729,7 +1873,7 @@
         <v>896</v>
       </c>
       <c r="F45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="2"/>
@@ -1881,7 +2025,7 @@
         <v>84</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
@@ -1907,7 +2051,7 @@
         <v>40</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="1"/>
@@ -1933,7 +2077,7 @@
         <v>84</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
@@ -1959,7 +2103,7 @@
         <v>40</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="1"/>
@@ -1985,7 +2129,7 @@
         <v>40</v>
       </c>
       <c r="F57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="1"/>
@@ -2011,7 +2155,7 @@
         <v>72</v>
       </c>
       <c r="F58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="1"/>
@@ -2037,7 +2181,7 @@
         <v>40</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="1"/>
@@ -2063,7 +2207,7 @@
         <v>68</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="1"/>
@@ -2089,7 +2233,7 @@
         <v>40</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="1"/>
@@ -2138,7 +2282,7 @@
         <v>16</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="1"/>
@@ -2187,7 +2331,7 @@
         <v>40</v>
       </c>
       <c r="F67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" si="1"/>
@@ -2213,7 +2357,7 @@
         <v>40</v>
       </c>
       <c r="F68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="1"/>
@@ -2262,10 +2406,10 @@
         <v>56</v>
       </c>
       <c r="F71" t="s">
+        <v>53</v>
+      </c>
+      <c r="G71" t="s">
         <v>54</v>
-      </c>
-      <c r="G71" t="s">
-        <v>55</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="1"/>
@@ -2291,10 +2435,10 @@
         <v>64</v>
       </c>
       <c r="F72" t="s">
+        <v>55</v>
+      </c>
+      <c r="G72" t="s">
         <v>56</v>
-      </c>
-      <c r="G72" t="s">
-        <v>57</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="1"/>
@@ -2325,7 +2469,7 @@
         <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
@@ -2365,9 +2509,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50946101-636E-4CAC-9348-8C1BCC50A424}">
-  <dimension ref="B1:L58"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -2376,7 +2520,10 @@
     <col min="6" max="6" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
       <c r="B1">
         <v>8</v>
       </c>
@@ -2403,7 +2550,10 @@
         <v>[InternalReferenceValue(8)] public Obj8[] Obj8s { get; set; }</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
       <c r="B2">
         <v>72</v>
       </c>
@@ -2430,7 +2580,10 @@
         <v>[InternalReferenceValue(72)] public Obj72[] Obj72s { get; set; }</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
       <c r="B3">
         <v>80</v>
       </c>
@@ -2457,7 +2610,10 @@
         <v>[InternalReferenceValue(80)] public Obj80[] Obj80s { get; set; }</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
       <c r="B4">
         <v>88</v>
       </c>
@@ -2484,7 +2640,10 @@
         <v>[InternalReferenceValue(88)] public Obj88[] Obj88s { get; set; }</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
       <c r="B5">
         <v>96</v>
       </c>
@@ -2511,7 +2670,10 @@
         <v>[InternalReferenceValue(96)] public Obj96[] Obj96s { get; set; }</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
       <c r="B6">
         <v>104</v>
       </c>
@@ -2538,7 +2700,10 @@
         <v>[InternalReferenceValue(104)] public Obj104[] Obj104s { get; set; }</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
       <c r="B7">
         <v>112</v>
       </c>
@@ -2553,7 +2718,7 @@
         <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
@@ -2564,7 +2729,10 @@
         <v>[InternalReferenceValue(112)] public Obj112[] Obj112s { get; set; }</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
       <c r="B8">
         <v>120</v>
       </c>
@@ -2591,7 +2759,10 @@
         <v>[InternalReferenceValue(120)] public Obj120[] Obj120s { get; set; }</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
       <c r="B9">
         <v>128</v>
       </c>
@@ -2618,7 +2789,10 @@
         <v>[InternalReferenceValue(128)] public Obj128[] Obj128s { get; set; }</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
       <c r="B10">
         <v>136</v>
       </c>
@@ -2633,7 +2807,7 @@
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
@@ -2644,7 +2818,10 @@
         <v>[InternalReferenceValue(136)] public Obj136[] Obj136s { get; set; }</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
       <c r="B11">
         <v>144</v>
       </c>
@@ -2671,7 +2848,10 @@
         <v>[InternalReferenceValue(144)] public Obj144[] Obj144s { get; set; }</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
       <c r="B12">
         <v>152</v>
       </c>
@@ -2686,7 +2866,7 @@
         <v>40</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="5"/>
+        <f>VLOOKUP(B12, MixedRefs,5, FALSE)</f>
         <v>Weap tag references, padded with zeroes</v>
       </c>
       <c r="H12" t="str">
@@ -2698,7 +2878,10 @@
         <v>[InternalReferenceValue(152)] public Obj152[] Obj152s { get; set; }</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
       <c r="B13">
         <v>160</v>
       </c>
@@ -2725,7 +2908,10 @@
         <v>[InternalReferenceValue(160)] public Obj160[] Obj160s { get; set; }</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
       <c r="B14">
         <v>168</v>
       </c>
@@ -2741,7 +2927,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="5"/>
-        <v>definitely sword placement on zanzibar - but not on lockout, no shotgun on lockout either</v>
+        <v>mach placement</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
@@ -2752,7 +2938,10 @@
         <v>[InternalReferenceValue(168)] public Obj168[] Obj168s { get; set; }</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
       <c r="B15">
         <v>176</v>
       </c>
@@ -2779,7 +2968,10 @@
         <v>[InternalReferenceValue(176)] public Obj176[] Obj176s { get; set; }</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
       <c r="B16">
         <v>184</v>
       </c>
@@ -2806,7 +2998,10 @@
         <v>[InternalReferenceValue(184)] public Obj184[] Obj184s { get; set; }</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
       <c r="B17">
         <v>192</v>
       </c>
@@ -2833,7 +3028,10 @@
         <v>[InternalReferenceValue(192)] public Obj192[] Obj192s { get; set; }</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
       <c r="B18">
         <v>216</v>
       </c>
@@ -2860,7 +3058,10 @@
         <v>[InternalReferenceValue(216)] public Obj216[] Obj216s { get; set; }</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
       <c r="B19">
         <v>224</v>
       </c>
@@ -2887,7 +3088,10 @@
         <v>[InternalReferenceValue(224)] public Obj224[] Obj224s { get; set; }</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
       <c r="B20">
         <v>232</v>
       </c>
@@ -2914,7 +3118,10 @@
         <v>[InternalReferenceValue(232)] public Obj232[] Obj232s { get; set; }</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
       <c r="B21">
         <v>240</v>
       </c>
@@ -2941,7 +3148,10 @@
         <v>[InternalReferenceValue(240)] public Obj240[] Obj240s { get; set; }</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
       <c r="B22">
         <v>248</v>
       </c>
@@ -2968,7 +3178,10 @@
         <v>[InternalReferenceValue(248)] public Obj248[] Obj248s { get; set; }</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
       <c r="B23">
         <v>256</v>
       </c>
@@ -2995,7 +3208,10 @@
         <v>[InternalReferenceValue(256)] public Obj256[] Obj256s { get; set; }</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
       <c r="B24">
         <v>264</v>
       </c>
@@ -3022,7 +3238,10 @@
         <v>[InternalReferenceValue(264)] public Obj264[] Obj264s { get; set; }</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
       <c r="B25">
         <v>304</v>
       </c>
@@ -3049,7 +3268,10 @@
         <v>[InternalReferenceValue(304)] public Obj304[] Obj304s { get; set; }</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
       <c r="B26">
         <v>312</v>
       </c>
@@ -3076,7 +3298,10 @@
         <v>[InternalReferenceValue(312)] public Obj312[] Obj312s { get; set; }</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
       <c r="B27">
         <v>320</v>
       </c>
@@ -3103,7 +3328,10 @@
         <v>[InternalReferenceValue(320)] public Obj320[] Obj320s { get; set; }</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
       <c r="B28">
         <v>336</v>
       </c>
@@ -3130,7 +3358,10 @@
         <v>[InternalReferenceValue(336)] public Obj336[] Obj336s { get; set; }</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
       <c r="B29">
         <v>344</v>
       </c>
@@ -3157,7 +3388,10 @@
         <v>[InternalReferenceValue(344)] public Obj344[] Obj344s { get; set; }</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
       <c r="B30">
         <v>352</v>
       </c>
@@ -3184,7 +3418,10 @@
         <v>[InternalReferenceValue(352)] public Obj352[] Obj352s { get; set; }</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
       <c r="B31">
         <v>360</v>
       </c>
@@ -3211,7 +3448,10 @@
         <v>[InternalReferenceValue(360)] public Obj360[] Obj360s { get; set; }</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
       <c r="B32">
         <v>368</v>
       </c>
@@ -3238,7 +3478,10 @@
         <v>[InternalReferenceValue(368)] public Obj368[] Obj368s { get; set; }</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
       <c r="B33">
         <v>376</v>
       </c>
@@ -3265,7 +3508,10 @@
         <v>[InternalReferenceValue(376)] public Obj376[] Obj376s { get; set; }</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
       <c r="B34">
         <v>432</v>
       </c>
@@ -3276,23 +3522,26 @@
         <v>359108</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E47" si="6">(D35-D34)/C34</f>
+        <f t="shared" ref="E34:E48" si="6">(D35-D34)/C34</f>
         <v>1.0000396683724067</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" ref="F34:F47" si="7">VLOOKUP(B34, MixedRefs,5, FALSE)</f>
+        <f t="shared" ref="F34:F48" si="7">VLOOKUP(B34, MixedRefs,5, FALSE)</f>
         <v>Text - looks like it would be used by scripts</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" ref="H34:H47" si="8">"[FixedLength(" &amp; E34 &amp; ")]public class Obj" &amp; B34 &amp; " {}"</f>
+        <f t="shared" ref="H34:H48" si="8">"[FixedLength(" &amp; E34 &amp; ")]public class Obj" &amp; B34 &amp; " {}"</f>
         <v>[FixedLength(1.00003966837241)]public class Obj432 {}</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" ref="L34:L47" si="9">"[InternalReferenceValue(" &amp; B34 &amp; ")] public Obj" &amp; B34 &amp; "[] Obj" &amp; B34 &amp; "s { get; set; }"</f>
+        <f t="shared" ref="L34:L48" si="9">"[InternalReferenceValue(" &amp; B34 &amp; ")] public Obj" &amp; B34 &amp; "[] Obj" &amp; B34 &amp; "s { get; set; }"</f>
         <v>[InternalReferenceValue(432)] public Obj432[] Obj432s { get; set; }</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
       <c r="B35">
         <v>440</v>
       </c>
@@ -3319,7 +3568,10 @@
         <v>[InternalReferenceValue(440)] public Obj440[] Obj440s { get; set; }</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
       <c r="B36">
         <v>448</v>
       </c>
@@ -3346,7 +3598,10 @@
         <v>[InternalReferenceValue(448)] public Obj448[] Obj448s { get; set; }</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
       <c r="B37">
         <v>456</v>
       </c>
@@ -3373,7 +3628,10 @@
         <v>[InternalReferenceValue(456)] public Obj456[] Obj456s { get; set; }</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
       <c r="B38">
         <v>472</v>
       </c>
@@ -3400,7 +3658,10 @@
         <v>[InternalReferenceValue(472)] public Obj472[] Obj472s { get; set; }</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
       <c r="B39">
         <v>480</v>
       </c>
@@ -3427,7 +3688,10 @@
         <v>[InternalReferenceValue(480)] public Obj480[] Obj480s { get; set; }</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
       <c r="B40">
         <v>496</v>
       </c>
@@ -3454,7 +3718,10 @@
         <v>[InternalReferenceValue(496)] public Obj496[] Obj496s { get; set; }</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
       <c r="B41">
         <v>528</v>
       </c>
@@ -3481,7 +3748,10 @@
         <v>[InternalReferenceValue(528)] public Obj528[] Obj528s { get; set; }</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
       <c r="B42">
         <v>536</v>
       </c>
@@ -3492,7 +3762,7 @@
         <v>436220</v>
       </c>
       <c r="E42">
-        <f t="shared" si="6"/>
+        <f>(D44-D42)/C42</f>
         <v>192</v>
       </c>
       <c r="F42" t="str">
@@ -3508,100 +3778,97 @@
         <v>[InternalReferenceValue(536)] public Obj536[] Obj536s { get; set; }</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
       <c r="B43">
+        <v>552</v>
+      </c>
+      <c r="F43" t="s">
+        <v>79</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="9"/>
+        <v>[InternalReferenceValue(552)] public Obj552[] Obj552s { get; set; }</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44">
         <v>560</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>1</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>436412</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="F43" t="str">
+      <c r="F44" t="str">
         <f t="shared" si="7"/>
         <v>Ids as shorts?</v>
       </c>
-      <c r="H43" t="str">
+      <c r="H44" t="str">
         <f t="shared" si="8"/>
         <v>[FixedLength(4)]public class Obj560 {}</v>
       </c>
-      <c r="L43" t="str">
+      <c r="L44" t="str">
         <f t="shared" si="9"/>
         <v>[InternalReferenceValue(560)] public Obj560[] Obj560s { get; set; }</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45">
         <v>568</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>27127</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>436416</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F45" t="str">
         <f t="shared" si="7"/>
         <v>Just 00, then 16 bytes of BA</v>
       </c>
-      <c r="H44" t="str">
+      <c r="H45" t="str">
         <f t="shared" si="8"/>
         <v>[FixedLength(20)]public class Obj568 {}</v>
       </c>
-      <c r="L44" t="str">
+      <c r="L45" t="str">
         <f t="shared" si="9"/>
         <v>[InternalReferenceValue(568)] public Obj568[] Obj568s { get; set; }</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46">
         <v>576</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>103</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>978956</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <f t="shared" si="6"/>
         <v>193.32038834951456</v>
-      </c>
-      <c r="F45" t="str">
-        <f t="shared" si="7"/>
-        <v>Strings like @352</v>
-      </c>
-      <c r="H45" t="str">
-        <f t="shared" si="8"/>
-        <v>[FixedLength(193.320388349515)]public class Obj576 {}</v>
-      </c>
-      <c r="L45" t="str">
-        <f t="shared" si="9"/>
-        <v>[InternalReferenceValue(576)] public Obj576[] Obj576s { get; set; }</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>584</v>
-      </c>
-      <c r="C46">
-        <v>44</v>
-      </c>
-      <c r="D46">
-        <v>998868</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="6"/>
-        <v>118</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="7"/>
@@ -3609,238 +3876,259 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="8"/>
-        <v>[FixedLength(118)]public class Obj584 {}</v>
+        <v>[FixedLength(193.320388349515)]public class Obj576 {}</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" si="9"/>
-        <v>[InternalReferenceValue(584)] public Obj584[] Obj584s { get; set; }</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+        <v>[InternalReferenceValue(576)] public Obj576[] Obj576s { get; set; }</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
       <c r="B47">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D47">
-        <v>1004060</v>
+        <v>998868</v>
       </c>
       <c r="E47">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="7"/>
-        <v>ascension string, then zeroes, then lsnd ref</v>
+        <v>Strings like @352</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="8"/>
-        <v>[FixedLength(100)]public class Obj592 {}</v>
+        <v>[FixedLength(118)]public class Obj584 {}</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="9"/>
-        <v>[InternalReferenceValue(592)] public Obj592[] Obj592s { get; set; }</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+        <v>[InternalReferenceValue(584)] public Obj584[] Obj584s { get; set; }</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>76</v>
+      </c>
       <c r="B48">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="C48">
         <v>5</v>
       </c>
       <c r="D48">
+        <v>1004060</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="7"/>
+        <v>ascension string, then zeroes, then lsnd ref</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="8"/>
+        <v>[FixedLength(100)]public class Obj592 {}</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="9"/>
+        <v>[InternalReferenceValue(592)] public Obj592[] Obj592s { get; set; }</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49">
+        <v>600</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
         <v>1004560</v>
       </c>
-      <c r="E48">
-        <f t="shared" ref="E48:E58" si="10">(D49-D48)/C48</f>
+      <c r="E49">
+        <f t="shared" ref="E49:E59" si="10">(D50-D49)/C49</f>
         <v>72</v>
       </c>
-      <c r="F48" t="str">
-        <f t="shared" ref="F48:F58" si="11">VLOOKUP(B48, MixedRefs,5, FALSE)</f>
+      <c r="F49" t="str">
+        <f t="shared" ref="F49:F59" si="11">VLOOKUP(B49, MixedRefs,5, FALSE)</f>
         <v>cliffs string, snde reference</v>
       </c>
-      <c r="H48" t="str">
-        <f t="shared" ref="H48:H58" si="12">"[FixedLength(" &amp; E48 &amp; ")]public class Obj" &amp; B48 &amp; " {}"</f>
+      <c r="H49" t="str">
+        <f t="shared" ref="H49:H59" si="12">"[FixedLength(" &amp; E49 &amp; ")]public class Obj" &amp; B49 &amp; " {}"</f>
         <v>[FixedLength(72)]public class Obj600 {}</v>
       </c>
-      <c r="L48" t="str">
-        <f t="shared" ref="L48:L58" si="13">"[InternalReferenceValue(" &amp; B48 &amp; ")] public Obj" &amp; B48 &amp; "[] Obj" &amp; B48 &amp; "s { get; set; }"</f>
+      <c r="L49" t="str">
+        <f t="shared" ref="L49:L59" si="13">"[InternalReferenceValue(" &amp; B49 &amp; ")] public Obj" &amp; B49 &amp; "[] Obj" &amp; B49 &amp; "s { get; set; }"</f>
         <v>[InternalReferenceValue(600)] public Obj600[] Obj600s { get; set; }</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50">
         <v>656</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>6</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>1004920</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <f t="shared" si="10"/>
         <v>1132.6666666666667</v>
       </c>
-      <c r="F49" t="str">
+      <c r="F50" t="str">
         <f t="shared" si="11"/>
         <v>Null sbsp tagref, internal refs to subsequent values (floats)</v>
       </c>
-      <c r="H49" t="str">
+      <c r="H50" t="str">
         <f t="shared" si="12"/>
         <v>[FixedLength(1132.66666666667)]public class Obj656 {}</v>
       </c>
-      <c r="L49" t="str">
+      <c r="L50" t="str">
         <f t="shared" si="13"/>
         <v>[InternalReferenceValue(656)] public Obj656[] Obj656s { get; set; }</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
         <v>792</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>1</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>1011716</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="F50" t="str">
+      <c r="F51" t="str">
         <f t="shared" si="11"/>
         <v>Internal refs, 48 size blocks, then more 48 size blocks. Lots of floats</v>
       </c>
-      <c r="H50" t="str">
+      <c r="H51" t="str">
         <f t="shared" si="12"/>
         <v>[FixedLength(96)]public class Obj792 {}</v>
       </c>
-      <c r="L50" t="str">
+      <c r="L51" t="str">
         <f t="shared" si="13"/>
         <v>[InternalReferenceValue(792)] public Obj792[] Obj792s { get; set; }</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52">
         <v>808</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>199</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <v>1011812</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <f t="shared" si="10"/>
         <v>76</v>
       </c>
-      <c r="F51" t="str">
+      <c r="F52" t="str">
         <f t="shared" si="11"/>
         <v>Crates and stuff</v>
       </c>
-      <c r="H51" t="str">
+      <c r="H52" t="str">
         <f t="shared" si="12"/>
         <v>[FixedLength(76)]public class Obj808 {}</v>
       </c>
-      <c r="L51" t="str">
+      <c r="L52" t="str">
         <f t="shared" si="13"/>
         <v>[InternalReferenceValue(808)] public Obj808[] Obj808s { get; set; }</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53">
         <v>816</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>27</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>1026936</v>
       </c>
-      <c r="E52">
+      <c r="E53">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="F52" t="str">
+      <c r="F53" t="str">
         <f t="shared" si="11"/>
         <v>bloc ref, padded with zeroes</v>
       </c>
-      <c r="H52" t="str">
+      <c r="H53" t="str">
         <f t="shared" si="12"/>
         <v>[FixedLength(40)]public class Obj816 {}</v>
       </c>
-      <c r="L52" t="str">
+      <c r="L53" t="str">
         <f t="shared" si="13"/>
         <v>[InternalReferenceValue(816)] public Obj816[] Obj816s { get; set; }</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B54">
         <v>832</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>1</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>1028016</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <f t="shared" si="10"/>
         <v>244</v>
       </c>
-      <c r="F53" t="str">
+      <c r="F54" t="str">
         <f t="shared" si="11"/>
         <v>Not sure, fpch ref? is that a tag?</v>
       </c>
-      <c r="H53" t="str">
+      <c r="H54" t="str">
         <f t="shared" si="12"/>
         <v>[FixedLength(244)]public class Obj832 {}</v>
       </c>
-      <c r="L53" t="str">
+      <c r="L54" t="str">
         <f t="shared" si="13"/>
         <v>[InternalReferenceValue(832)] public Obj832[] Obj832s { get; set; }</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B55">
         <v>888</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>2</v>
       </c>
-      <c r="D54">
+      <c r="D55">
         <v>1028260</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-      <c r="F54" t="str">
-        <f t="shared" si="11"/>
-        <v>DECR refs</v>
-      </c>
-      <c r="H54" t="str">
-        <f t="shared" si="12"/>
-        <v>[FixedLength(8)]public class Obj888 {}</v>
-      </c>
-      <c r="L54" t="str">
-        <f t="shared" si="13"/>
-        <v>[InternalReferenceValue(888)] public Obj888[] Obj888s { get; set; }</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>896</v>
-      </c>
-      <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="D55">
-        <v>1028276</v>
       </c>
       <c r="E55">
         <f t="shared" si="10"/>
@@ -3848,99 +4136,143 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="11"/>
-        <v>Some shorts</v>
+        <v>DECR refs</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="12"/>
-        <v>[FixedLength(8)]public class Obj896 {}</v>
+        <v>[FixedLength(8)]public class Obj888 {}</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="13"/>
-        <v>[InternalReferenceValue(896)] public Obj896[] Obj896s { get; set; }</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+        <v>[InternalReferenceValue(888)] public Obj888[] Obj888s { get; set; }</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D56">
-        <v>1028300</v>
+        <v>1028276</v>
       </c>
       <c r="E56">
         <f t="shared" si="10"/>
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="11"/>
-        <v>Empty sbsp ref</v>
+        <v>Some shorts</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="12"/>
-        <v>[FixedLength(34)]public class Obj904 {}</v>
+        <v>[FixedLength(8)]public class Obj896 {}</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="13"/>
-        <v>[InternalReferenceValue(904)] public Obj904[] Obj904s { get; set; }</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+        <v>[InternalReferenceValue(896)] public Obj896[] Obj896s { get; set; }</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
       <c r="B57">
-        <v>920</v>
+        <v>904</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D57">
-        <v>1028504</v>
+        <v>1028300</v>
       </c>
       <c r="E57">
         <f t="shared" si="10"/>
-        <v>2920</v>
+        <v>34</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="11"/>
-        <v>Bitm, then utf-16 strings of the name and description of the map</v>
+        <v>Empty sbsp ref</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="12"/>
-        <v>[FixedLength(2920)]public class Obj920 {}</v>
+        <v>[FixedLength(34)]public class Obj904 {}</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="13"/>
-        <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+        <v>[InternalReferenceValue(904)] public Obj904[] Obj904s { get; set; }</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
       <c r="B58">
-        <v>984</v>
+        <v>920</v>
       </c>
       <c r="C58">
-        <v>428</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>1031424</v>
+        <v>1028504</v>
       </c>
       <c r="E58">
         <f t="shared" si="10"/>
-        <v>-2409.8691588785045</v>
+        <v>2920</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="11"/>
-        <v>Shorts referencing the current raw offset. Padding for future changes to prevent recalculating magics?</v>
+        <v>Bitm, then utf-16 strings of the name and description of the map</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="12"/>
-        <v>[FixedLength(-2409.8691588785)]public class Obj984 {}</v>
+        <v>[FixedLength(2920)]public class Obj920 {}</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="13"/>
+        <v>[InternalReferenceValue(920)] public Obj920[] Obj920s { get; set; }</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>984</v>
+      </c>
+      <c r="C59">
+        <v>428</v>
+      </c>
+      <c r="D59">
+        <v>1031424</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="10"/>
+        <v>-2409.8691588785045</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="11"/>
+        <v>Shorts referencing the current raw offset. Padding for future changes to prevent recalculating magics?</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="12"/>
+        <v>[FixedLength(-2409.8691588785)]public class Obj984 {}</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="13"/>
         <v>[InternalReferenceValue(984)] public Obj984[] Obj984s { get; set; }</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A59">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"''"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3950,8 +4282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A61BE83-A9AA-4FA7-880A-944707CC9C14}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:C58"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4598,4 +4930,154 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E2CD54-8002-4905-B0AC-525BD08EFB2E}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="78.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working towards physics implementation
</commit_message>
<xml_diff>
--- a/doc/Research/ScenarioResearch.xlsx
+++ b/doc/Research/ScenarioResearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronal\source\openh2\doc\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F124A0C7-275F-43DA-814C-EE35F9617AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50435389-3673-48A2-999B-AE2EAC161C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
   <si>
     <t>Cao Location</t>
   </si>
@@ -318,6 +318,9 @@
     <t>ValueJ</t>
   </si>
   <si>
+    <t>next</t>
+  </si>
+  <si>
     <t>next node</t>
   </si>
   <si>
@@ -367,6 +370,15 @@
   </si>
   <si>
     <t>Some lower values, but mostly 32k and up, maybe separate byte vals</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>previous check</t>
+  </si>
+  <si>
+    <t>string position</t>
   </si>
 </sst>
 </file>
@@ -2511,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50946101-636E-4CAC-9348-8C1BCC50A424}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -4934,147 +4946,166 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E2CD54-8002-4905-B0AC-525BD08EFB2E}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="78.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>87</v>
       </c>
       <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>